<commit_message>
changed layout of utilization tab
</commit_message>
<xml_diff>
--- a/ShinyApp/data/demographics-loudoun.xlsx
+++ b/ShinyApp/data/demographics-loudoun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2110EDC7-42DD-8140-8B7D-57D4EF50EAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D71675E-88C0-D342-B36D-27F23D3AFDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="15440" xr2:uid="{1C34EB15-CE9B-2A4C-B502-CCE8971AB6FD}"/>
   </bookViews>
@@ -42,15 +42,9 @@
     <t>Black</t>
   </si>
   <si>
-    <t>Indian</t>
-  </si>
-  <si>
     <t>Asian</t>
   </si>
   <si>
-    <t>Native Hawaiian</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -136,13 +130,19 @@
   </si>
   <si>
     <t>Undisclosed Gender</t>
+  </si>
+  <si>
+    <t>American Indian/Alaska Native</t>
+  </si>
+  <si>
+    <t>Native Hawai’ian/Pacific Islander</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,6 +152,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -178,9 +185,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,53 +503,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F761564-6FFA-9A47-8265-8EA128649961}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="16" max="16" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -552,31 +561,31 @@
         <v>20066</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1">
         <v>1473</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2">
         <v>396</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K2">
         <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N2">
         <v>9</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q2">
         <v>180</v>
@@ -590,31 +599,31 @@
         <v>2403</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1">
         <v>25418</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3">
         <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N3">
         <v>5</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q3">
         <v>30</v>
@@ -622,19 +631,19 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H4">
         <v>49</v>
@@ -646,13 +655,13 @@
         <v>10</v>
       </c>
       <c r="M4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N4">
         <v>61.3</v>
       </c>
       <c r="P4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q4">
         <v>75</v>
@@ -660,37 +669,37 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>3891</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K5">
         <v>6</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N5">
         <v>79.599999999999994</v>
       </c>
       <c r="P5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q5">
         <v>23</v>
@@ -698,25 +707,25 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H6">
         <v>105</v>
       </c>
       <c r="M6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N6">
         <v>12.1</v>
       </c>
       <c r="P6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q6">
         <v>2</v>
@@ -724,13 +733,13 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>425</v>
       </c>
       <c r="P7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q7">
         <v>17</v>
@@ -738,11 +747,14 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q8">
         <v>11</v>
       </c>
+    </row>
+    <row r="12" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed trees section and added 2 more programs.
</commit_message>
<xml_diff>
--- a/ShinyApp/data/demographics-loudoun.xlsx
+++ b/ShinyApp/data/demographics-loudoun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D71675E-88C0-D342-B36D-27F23D3AFDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BF09B1-1094-E143-95A3-DFFE8FA1C432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="15440" xr2:uid="{1C34EB15-CE9B-2A4C-B502-CCE8971AB6FD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>White</t>
   </si>
@@ -136,6 +136,36 @@
   </si>
   <si>
     <t>Native Hawai’ian/Pacific Islander</t>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">families' lights on </t>
+  </si>
+  <si>
+    <t>rental and utility assistance</t>
+  </si>
+  <si>
+    <t>didn’t not qualify for government support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">client records </t>
+  </si>
+  <si>
+    <t xml:space="preserve">residents </t>
+  </si>
+  <si>
+    <t>at 70% of below AMI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hispanic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spanish Speakers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">at 70% or below median income </t>
   </si>
 </sst>
 </file>
@@ -185,10 +215,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,19 +534,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F761564-6FFA-9A47-8265-8EA128649961}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="16" max="16" width="18.83203125" customWidth="1"/>
+    <col min="20" max="20" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -552,8 +584,14 @@
       <c r="Q1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -590,8 +628,14 @@
       <c r="Q2">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S2">
+        <v>540</v>
+      </c>
+      <c r="T2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -628,8 +672,14 @@
       <c r="Q3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S3" s="3">
+        <v>900000</v>
+      </c>
+      <c r="T3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -666,8 +716,14 @@
       <c r="Q4">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <v>55</v>
+      </c>
+      <c r="T4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -681,10 +737,10 @@
         <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
@@ -704,8 +760,14 @@
       <c r="Q5">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <v>1290</v>
+      </c>
+      <c r="T5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -713,10 +775,10 @@
         <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="M6" t="s">
         <v>24</v>
@@ -730,8 +792,14 @@
       <c r="Q6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S6">
+        <v>3999</v>
+      </c>
+      <c r="T6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -744,16 +812,44 @@
       <c r="Q7">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <v>95</v>
+      </c>
+      <c r="T7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="P8" t="s">
         <v>30</v>
       </c>
       <c r="Q8">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <v>79.8</v>
+      </c>
+      <c r="T8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S9">
+        <v>74.3</v>
+      </c>
+      <c r="T9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <v>95</v>
+      </c>
+      <c r="T10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="20" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ethnicity graph for tays and part of provision bullet.
</commit_message>
<xml_diff>
--- a/ShinyApp/data/demographics-loudoun.xlsx
+++ b/ShinyApp/data/demographics-loudoun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BF09B1-1094-E143-95A3-DFFE8FA1C432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE0EAF9-B4FE-7943-B5AF-5EE284B4D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="15440" xr2:uid="{1C34EB15-CE9B-2A4C-B502-CCE8971AB6FD}"/>
   </bookViews>
@@ -141,31 +141,31 @@
     <t>Stat</t>
   </si>
   <si>
-    <t xml:space="preserve">families' lights on </t>
-  </si>
-  <si>
-    <t>rental and utility assistance</t>
-  </si>
-  <si>
-    <t>didn’t not qualify for government support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client records </t>
-  </si>
-  <si>
-    <t xml:space="preserve">residents </t>
-  </si>
-  <si>
-    <t>at 70% of below AMI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spanish Speakers </t>
-  </si>
-  <si>
-    <t xml:space="preserve">at 70% or below median income </t>
+    <t>Hispanic (%)</t>
+  </si>
+  <si>
+    <t>Spanish Speakers (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Families' lights on </t>
+  </si>
+  <si>
+    <t>Rental and utility assistance (K)</t>
+  </si>
+  <si>
+    <t>Didn’t not qualify for government support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client records </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residents </t>
+  </si>
+  <si>
+    <t>70% of below AMI (%)</t>
+  </si>
+  <si>
+    <t>70% or below median income (%)</t>
   </si>
 </sst>
 </file>
@@ -536,15 +536,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F761564-6FFA-9A47-8265-8EA128649961}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="16" max="16" width="18.83203125" customWidth="1"/>
-    <col min="20" max="20" width="25.33203125" customWidth="1"/>
+    <col min="20" max="20" width="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -632,7 +632,7 @@
         <v>540</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -673,10 +673,10 @@
         <v>30</v>
       </c>
       <c r="S3" s="3">
-        <v>900000</v>
+        <v>900</v>
       </c>
       <c r="T3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -720,7 +720,7 @@
         <v>55</v>
       </c>
       <c r="T4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -764,7 +764,7 @@
         <v>1290</v>
       </c>
       <c r="T5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>3999</v>
       </c>
       <c r="T6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
         <v>95</v>
       </c>
       <c r="T7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -827,26 +827,26 @@
         <v>11</v>
       </c>
       <c r="S8">
-        <v>79.8</v>
+        <v>95</v>
       </c>
       <c r="T8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="S9">
-        <v>74.3</v>
+        <v>79.8</v>
       </c>
       <c r="T9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="S10">
-        <v>95</v>
+        <v>74.3</v>
       </c>
       <c r="T10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed popups for utilization tab and changed layout of family services
</commit_message>
<xml_diff>
--- a/ShinyApp/data/demographics-loudoun.xlsx
+++ b/ShinyApp/data/demographics-loudoun.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6362A0-5ABA-C241-B334-EFD8957108AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22A0DCF-371D-E347-B85C-E445CA2D7D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="15440" xr2:uid="{1C34EB15-CE9B-2A4C-B502-CCE8971AB6FD}"/>
+    <workbookView xWindow="8080" yWindow="2000" windowWidth="20340" windowHeight="15440" xr2:uid="{1C34EB15-CE9B-2A4C-B502-CCE8971AB6FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>White</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>70% or below median income (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F761564-6FFA-9A47-8265-8EA128649961}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,7 +550,7 @@
     <col min="20" max="20" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -590,8 +593,14 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -634,8 +643,14 @@
       <c r="T2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V2">
+        <v>2016</v>
+      </c>
+      <c r="W2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -678,8 +693,14 @@
       <c r="T3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V3">
+        <v>2017</v>
+      </c>
+      <c r="W3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -722,8 +743,14 @@
       <c r="T4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V4">
+        <v>2018</v>
+      </c>
+      <c r="W4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -766,8 +793,14 @@
       <c r="T5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V5">
+        <v>2019</v>
+      </c>
+      <c r="W5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -798,8 +831,14 @@
       <c r="T6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V6">
+        <v>2020</v>
+      </c>
+      <c r="W6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -819,7 +858,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="P8" t="s">
         <v>30</v>
       </c>
@@ -833,7 +872,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="S9">
         <v>79.8</v>
       </c>
@@ -841,7 +880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="S10">
         <v>74.3</v>
       </c>
@@ -849,7 +888,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="20" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
   </sheetData>

</xml_diff>